<commit_message>
added code to track reduced reserves by generator.
</commit_message>
<xml_diff>
--- a/model_outputs/analysis_water_failure/water_deficit_pipe_1.xlsx
+++ b/model_outputs/analysis_water_failure/water_deficit_pipe_1.xlsx
@@ -6725,6 +6725,65 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Water demand </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6744,7 +6803,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -6786,6 +6845,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Total system deficit (GPM)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6805,7 +6917,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -6820,6 +6932,7 @@
         <c:crossAx val="496572984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -6844,7 +6957,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -7796,7 +7909,7 @@
   <dimension ref="A1:D502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>